<commit_message>
added reload score function
</commit_message>
<xml_diff>
--- a/public/uploads/amd_scoresheet_wolfvilleacadia.xlsx
+++ b/public/uploads/amd_scoresheet_wolfvilleacadia.xlsx
@@ -161,7 +161,7 @@
     <numFmt numFmtId="168" formatCode="0.000"/>
     <numFmt numFmtId="169" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -229,13 +229,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -244,18 +237,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor rgb="FFFCD5B5"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -266,7 +253,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFCD5B5"/>
-        <bgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
     <fill>
@@ -276,7 +263,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="33">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -285,13 +272,150 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
       <right/>
-      <top style="thin">
-        <color rgb="FF4F81BD"/>
-      </top>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="medium"/>
       <bottom style="double">
         <color rgb="FF4F81BD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="double">
+        <color rgb="FF4F81BD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="double">
+        <color rgb="FF4F81BD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="double">
+        <color rgb="FF4F81BD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -320,154 +444,6 @@
       <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="double">
-        <color rgb="FF4F81BD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="double">
-        <color rgb="FF4F81BD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="double">
-        <color rgb="FF4F81BD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="double">
-        <color rgb="FF4F81BD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -578,7 +554,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -602,13 +578,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="3" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -633,135 +603,139 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="14" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="4" borderId="20" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="4" borderId="2" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="3" borderId="21" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="11" fillId="3" borderId="22" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="11" fillId="3" borderId="3" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="11" fillId="3" borderId="25" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="2" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="10" fillId="2" borderId="21" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="10" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="10" fillId="2" borderId="24" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="4" borderId="29" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="29" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -769,37 +743,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="11" fillId="3" borderId="32" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="11" fillId="3" borderId="33" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="4" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="10" fillId="2" borderId="31" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="10" fillId="2" borderId="32" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Total" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Input" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Output" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -821,7 +789,7 @@
       <rgbColor rgb="FF7F7F7F"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFCD5B5"/>
+      <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFDBEEF4"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -842,7 +810,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFCD5B5"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -857,7 +825,7 @@
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF3F3F76"/>
+      <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF3F3F3F"/>
     </indexedColors>
   </colors>
@@ -872,7 +840,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1123,12 +1091,12 @@
       </c>
       <c r="L7" s="31" t="n">
         <f aca="false">RANK(K7, $K$5:$K$19)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M7" s="38"/>
       <c r="N7" s="39"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="33" t="s">
         <v>25</v>
       </c>
@@ -1150,7 +1118,7 @@
         <v>31.2</v>
       </c>
       <c r="G8" s="26" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H8" s="27" t="n">
         <v>31</v>
@@ -1161,15 +1129,15 @@
       </c>
       <c r="J8" s="42" t="n">
         <f aca="false">IF(ISBLANK(H8),G8,IF(I8&gt;=1,G8-32,G8-30*I8))</f>
-        <v>0.0292860809240523</v>
+        <v>20.0292860809241</v>
       </c>
       <c r="K8" s="30" t="n">
         <f aca="false">AVERAGE(F8,J8)</f>
-        <v>15.614643040462</v>
+        <v>25.614643040462</v>
       </c>
       <c r="L8" s="31" t="n">
         <f aca="false">RANK(K8, $K$5:$K$19)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M8" s="31"/>
       <c r="N8" s="32"/>
@@ -1181,33 +1149,41 @@
       <c r="B9" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="24" t="str">
+      <c r="C9" s="22" t="n">
+        <v>60</v>
+      </c>
+      <c r="D9" s="40" t="n">
+        <v>20000</v>
+      </c>
+      <c r="E9" s="24" t="n">
         <f aca="false">IF(ISBLANK(D9),"no data",TRUNC(ABS($E$2-D9)/$E$2,2))</f>
-        <v>no data</v>
+        <v>0.37</v>
       </c>
       <c r="F9" s="25" t="n">
         <f aca="false">IF(ISBLANK(D9),C9,IF(E9&gt;=1,C9-32,C9-30*E9))</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="26"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="41" t="str">
+        <v>48.9</v>
+      </c>
+      <c r="G9" s="26" t="n">
+        <v>70</v>
+      </c>
+      <c r="H9" s="27" t="n">
+        <v>20</v>
+      </c>
+      <c r="I9" s="41" t="n">
         <f aca="false">IF(ISBLANK(H9),"no data",ABS($I$2-H9)/$I$2)</f>
-        <v>no data</v>
+        <v>0.999370191808085</v>
       </c>
       <c r="J9" s="42" t="n">
         <f aca="false">IF(ISBLANK(H9),G9,IF(I9&gt;=1,G9-32,G9-30*I9))</f>
-        <v>0</v>
+        <v>40.0188942457575</v>
       </c>
       <c r="K9" s="30" t="n">
         <f aca="false">AVERAGE(F9,J9)</f>
-        <v>0</v>
+        <v>44.4594471228787</v>
       </c>
       <c r="L9" s="31" t="n">
         <f aca="false">RANK(K9, $K$5:$K$19)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M9" s="31"/>
       <c r="N9" s="32"/>
@@ -1245,7 +1221,7 @@
       </c>
       <c r="L10" s="31" t="n">
         <f aca="false">RANK(K10, $K$5:$K$19)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M10" s="31"/>
       <c r="N10" s="32"/>
@@ -1283,7 +1259,7 @@
       </c>
       <c r="L11" s="31" t="n">
         <f aca="false">RANK(K11, $K$5:$K$19)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M11" s="31"/>
       <c r="N11" s="32"/>
@@ -1321,7 +1297,7 @@
       </c>
       <c r="L12" s="31" t="n">
         <f aca="false">RANK(K12, $K$5:$K$19)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M12" s="31"/>
       <c r="N12" s="32"/>
@@ -1359,7 +1335,7 @@
       </c>
       <c r="L13" s="31" t="n">
         <f aca="false">RANK(K13, $K$5:$K$19)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M13" s="31"/>
       <c r="N13" s="32"/>
@@ -1397,7 +1373,7 @@
       </c>
       <c r="L14" s="31" t="n">
         <f aca="false">RANK(K14, $K$5:$K$19)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M14" s="31"/>
       <c r="N14" s="32"/>
@@ -1435,7 +1411,7 @@
       </c>
       <c r="L15" s="31" t="n">
         <f aca="false">RANK(K15, $K$5:$K$19)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M15" s="31"/>
       <c r="N15" s="32"/>
@@ -1473,7 +1449,7 @@
       </c>
       <c r="L16" s="31" t="n">
         <f aca="false">RANK(K16, $K$5:$K$19)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M16" s="31"/>
       <c r="N16" s="32"/>
@@ -1511,7 +1487,7 @@
       </c>
       <c r="L17" s="31" t="n">
         <f aca="false">RANK(K17, $K$5:$K$19)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M17" s="31"/>
       <c r="N17" s="32"/>
@@ -1549,7 +1525,7 @@
       </c>
       <c r="L18" s="31" t="n">
         <f aca="false">RANK(K18, $K$5:$K$19)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M18" s="31"/>
       <c r="N18" s="32"/>
@@ -1587,7 +1563,7 @@
       </c>
       <c r="L19" s="31" t="n">
         <f aca="false">RANK(K19, $K$5:$K$19)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M19" s="31"/>
       <c r="N19" s="32"/>

</xml_diff>